<commit_message>
Committing everything just cause
</commit_message>
<xml_diff>
--- a/project/data/DT_out/analysis.xlsx
+++ b/project/data/DT_out/analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Equal-Equal Size of Forest Test</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>SkewedSkewed</t>
+  </si>
+  <si>
+    <t>Percent of Training Set</t>
   </si>
 </sst>
 </file>
@@ -91,8 +94,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -147,7 +164,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -173,6 +190,13 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -198,6 +222,13 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,7 +943,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$35</c:f>
+              <c:f>Sheet1!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -923,7 +954,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$36:$A$46</c:f>
+              <c:f>Sheet1!$A$27:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -965,7 +996,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$36:$C$46</c:f>
+              <c:f>Sheet1!$C$27:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1012,7 +1043,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$35</c:f>
+              <c:f>Sheet1!$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1023,7 +1054,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$36:$A$46</c:f>
+              <c:f>Sheet1!$A$27:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1065,7 +1096,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$36:$D$46</c:f>
+              <c:f>Sheet1!$D$27:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1112,7 +1143,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$35</c:f>
+              <c:f>Sheet1!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1123,7 +1154,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$36:$A$46</c:f>
+              <c:f>Sheet1!$A$27:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1165,7 +1196,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$36:$E$46</c:f>
+              <c:f>Sheet1!$E$27:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1212,7 +1243,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$35</c:f>
+              <c:f>Sheet1!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1223,7 +1254,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$36:$A$46</c:f>
+              <c:f>Sheet1!$A$27:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1265,7 +1296,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$B$46</c:f>
+              <c:f>Sheet1!$B$27:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1419,6 +1450,406 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Metrics on Random</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Forest, Original Data, vs Percent of Training Sample Used</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$16:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$16:$R$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.983388228555062</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.980667334956322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.977087211800086</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.985679507375053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$16:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$16:$S$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.698929036132519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.703946694003075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.707291881842594</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.707486520116134</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.707327098962079</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$16:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$16:$T$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.822787793095322</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.820528139562671</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.821842184218421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.820713297648403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.823620916596864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$16:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$16:$Q$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.698929036132519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.699329396456811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.702832549294364</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.701631468321489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.704934440996897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2077488632"/>
+        <c:axId val="2039033240"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2077488632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent of Training Sample Used (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2039033240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2039033240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+          <c:min val="0.65"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Metric Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077488632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1429,10 +1860,10 @@
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1454,15 +1885,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1476,6 +1907,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1806,15 +2267,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A12:F46"/>
+  <dimension ref="A12:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +2295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1854,7 +2315,7 @@
         <v>0.72780707061975902</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1874,7 +2335,7 @@
         <v>0.73852701200834803</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1893,8 +2354,26 @@
       <c r="F15">
         <v>0.752415175897716</v>
       </c>
+      <c r="P15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>3</v>
+      </c>
+      <c r="S15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1913,8 +2392,26 @@
       <c r="F16">
         <v>0.75025730630220899</v>
       </c>
+      <c r="P16">
+        <v>25</v>
+      </c>
+      <c r="Q16">
+        <v>0.698929036132519</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0.698929036132519</v>
+      </c>
+      <c r="T16">
+        <v>0.82278779309532202</v>
+      </c>
+      <c r="U16">
+        <v>0.74371099324770396</v>
+      </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>21</v>
       </c>
@@ -1933,8 +2430,26 @@
       <c r="F17">
         <v>0.74933822032172603</v>
       </c>
+      <c r="P17">
+        <v>50</v>
+      </c>
+      <c r="Q17">
+        <v>0.69932939645681103</v>
+      </c>
+      <c r="R17">
+        <v>0.98338822855506203</v>
+      </c>
+      <c r="S17">
+        <v>0.70394669400307497</v>
+      </c>
+      <c r="T17">
+        <v>0.82052813956267101</v>
+      </c>
+      <c r="U17">
+        <v>0.74636436754124702</v>
+      </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>51</v>
       </c>
@@ -1953,8 +2468,26 @@
       <c r="F18">
         <v>0.74822888283378697</v>
       </c>
+      <c r="P18">
+        <v>100</v>
+      </c>
+      <c r="Q18">
+        <v>0.70283254929436401</v>
+      </c>
+      <c r="R18">
+        <v>0.98066733495632197</v>
+      </c>
+      <c r="S18">
+        <v>0.70729188184259395</v>
+      </c>
+      <c r="T18">
+        <v>0.82184218421842103</v>
+      </c>
+      <c r="U18">
+        <v>0.74905383824462302</v>
+      </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>101</v>
       </c>
@@ -1973,8 +2506,26 @@
       <c r="F19">
         <v>0.74897110380419396</v>
       </c>
+      <c r="P19">
+        <v>200</v>
+      </c>
+      <c r="Q19">
+        <v>0.70163146832148904</v>
+      </c>
+      <c r="R19">
+        <v>0.97708721180008595</v>
+      </c>
+      <c r="S19">
+        <v>0.707486520116134</v>
+      </c>
+      <c r="T19">
+        <v>0.82071329764840295</v>
+      </c>
+      <c r="U19">
+        <v>0.74880923637481001</v>
+      </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>201</v>
       </c>
@@ -1993,8 +2544,26 @@
       <c r="F20">
         <v>0.74520002568548105</v>
       </c>
+      <c r="P20">
+        <v>400</v>
+      </c>
+      <c r="Q20">
+        <v>0.70493444099689695</v>
+      </c>
+      <c r="R20">
+        <v>0.98567950737505305</v>
+      </c>
+      <c r="S20">
+        <v>0.70732709896207902</v>
+      </c>
+      <c r="T20">
+        <v>0.82362091659686398</v>
+      </c>
+      <c r="U20">
+        <v>0.74966780665258004</v>
+      </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>301</v>
       </c>
@@ -2014,7 +2583,7 @@
         <v>0.74392140984933997</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:21">
       <c r="A22">
         <v>401</v>
       </c>
@@ -2034,7 +2603,7 @@
         <v>0.74371099324770396</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:21">
       <c r="A23">
         <v>501</v>
       </c>
@@ -2054,243 +2623,243 @@
         <v>0.74371099324770396</v>
       </c>
     </row>
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0.56743721935805702</v>
+      </c>
+      <c r="C27">
+        <v>0.55038244097106703</v>
+      </c>
+      <c r="D27">
+        <v>0.56990358126721696</v>
+      </c>
+      <c r="E27">
+        <v>0.55997293182202601</v>
+      </c>
+      <c r="F27">
+        <v>0.56588935239006999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28">
+        <v>101</v>
+      </c>
+      <c r="B28">
+        <v>0.59288208880758297</v>
+      </c>
+      <c r="C28">
+        <v>0.56634519454605903</v>
+      </c>
+      <c r="D28">
+        <v>0.59817351598173496</v>
+      </c>
+      <c r="E28">
+        <v>0.58182439357704097</v>
+      </c>
+      <c r="F28">
+        <v>0.59152483501215702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29">
+        <v>201</v>
+      </c>
+      <c r="B29">
+        <v>0.59454515217029702</v>
+      </c>
+      <c r="C29">
+        <v>0.50049883604921797</v>
+      </c>
+      <c r="D29">
+        <v>0.61655059401884404</v>
+      </c>
+      <c r="E29">
+        <v>0.55249632892804701</v>
+      </c>
+      <c r="F29">
+        <v>0.58922558922558899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30">
+        <v>301</v>
+      </c>
+      <c r="B30">
+        <v>0.58889073673706904</v>
+      </c>
+      <c r="C30">
+        <v>0.54705686730961001</v>
+      </c>
+      <c r="D30">
+        <v>0.59709618874773096</v>
+      </c>
+      <c r="E30">
+        <v>0.57098229781325904</v>
+      </c>
+      <c r="F30">
+        <v>0.586369145219933</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31">
+        <v>401</v>
+      </c>
+      <c r="B31">
+        <v>0.58440046565774095</v>
+      </c>
+      <c r="C31">
+        <v>0.49916860658463502</v>
+      </c>
+      <c r="D31">
+        <v>0.60184442662389703</v>
+      </c>
+      <c r="E31">
+        <v>0.54571896018905597</v>
+      </c>
+      <c r="F31">
+        <v>0.57806362165909198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32">
+        <v>501</v>
+      </c>
+      <c r="B32">
+        <v>0.61051056045235297</v>
+      </c>
+      <c r="C32">
+        <v>0.512138343864316</v>
+      </c>
+      <c r="D32">
+        <v>0.63768115942028902</v>
+      </c>
+      <c r="E32">
+        <v>0.56805606787163399</v>
+      </c>
+      <c r="F32">
+        <v>0.60787874003315601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>601</v>
+      </c>
+      <c r="B33">
+        <v>0.62714119407949398</v>
+      </c>
+      <c r="C33">
+        <v>0.66012637179913503</v>
+      </c>
+      <c r="D33">
+        <v>0.61934477379095099</v>
+      </c>
+      <c r="E33">
+        <v>0.63908564069542795</v>
+      </c>
+      <c r="F33">
+        <v>0.62709294244013403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>701</v>
+      </c>
+      <c r="B34">
+        <v>0.62431398636288005</v>
+      </c>
+      <c r="C34">
+        <v>0.55404057199866896</v>
+      </c>
+      <c r="D34">
+        <v>0.64473684210526305</v>
+      </c>
+      <c r="E34">
+        <v>0.59595778930423804</v>
+      </c>
+      <c r="F34">
+        <v>0.62429738439631199</v>
+      </c>
+    </row>
     <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
+      <c r="A35">
+        <v>801</v>
+      </c>
+      <c r="B35">
+        <v>0.634458672875436</v>
+      </c>
+      <c r="C35">
+        <v>0.61157299634186901</v>
+      </c>
+      <c r="D35">
+        <v>0.64098989194841405</v>
+      </c>
+      <c r="E35">
+        <v>0.62593601089176298</v>
+      </c>
+      <c r="F35">
+        <v>0.63488227577159395</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>1</v>
+        <v>901</v>
       </c>
       <c r="B36">
-        <v>0.56743721935805702</v>
+        <v>0.63894894395476398</v>
       </c>
       <c r="C36">
-        <v>0.55038244097106703</v>
+        <v>0.60226139008978996</v>
       </c>
       <c r="D36">
-        <v>0.56990358126721696</v>
+        <v>0.650035893754486</v>
       </c>
       <c r="E36">
-        <v>0.55997293182202601</v>
+        <v>0.62523735542896597</v>
       </c>
       <c r="F36">
-        <v>0.56588935239006999</v>
+        <v>0.63988410713023802</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>101</v>
+        <v>1001</v>
       </c>
       <c r="B37">
-        <v>0.59288208880758297</v>
+        <v>0.58040911358722702</v>
       </c>
       <c r="C37">
-        <v>0.56634519454605903</v>
+        <v>0.27302959760558698</v>
       </c>
       <c r="D37">
-        <v>0.59817351598173496</v>
+        <v>0.70898100172711498</v>
       </c>
       <c r="E37">
-        <v>0.58182439357704097</v>
+        <v>0.39423769507803103</v>
       </c>
       <c r="F37">
-        <v>0.59152483501215702</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>201</v>
-      </c>
-      <c r="B38">
-        <v>0.59454515217029702</v>
-      </c>
-      <c r="C38">
-        <v>0.50049883604921797</v>
-      </c>
-      <c r="D38">
-        <v>0.61655059401884404</v>
-      </c>
-      <c r="E38">
-        <v>0.55249632892804701</v>
-      </c>
-      <c r="F38">
-        <v>0.58922558922558899</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39">
-        <v>301</v>
-      </c>
-      <c r="B39">
-        <v>0.58889073673706904</v>
-      </c>
-      <c r="C39">
-        <v>0.54705686730961001</v>
-      </c>
-      <c r="D39">
-        <v>0.59709618874773096</v>
-      </c>
-      <c r="E39">
-        <v>0.57098229781325904</v>
-      </c>
-      <c r="F39">
-        <v>0.586369145219933</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>401</v>
-      </c>
-      <c r="B40">
-        <v>0.58440046565774095</v>
-      </c>
-      <c r="C40">
-        <v>0.49916860658463502</v>
-      </c>
-      <c r="D40">
-        <v>0.60184442662389703</v>
-      </c>
-      <c r="E40">
-        <v>0.54571896018905597</v>
-      </c>
-      <c r="F40">
-        <v>0.57806362165909198</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>501</v>
-      </c>
-      <c r="B41">
-        <v>0.61051056045235297</v>
-      </c>
-      <c r="C41">
-        <v>0.512138343864316</v>
-      </c>
-      <c r="D41">
-        <v>0.63768115942028902</v>
-      </c>
-      <c r="E41">
-        <v>0.56805606787163399</v>
-      </c>
-      <c r="F41">
-        <v>0.60787874003315601</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>601</v>
-      </c>
-      <c r="B42">
-        <v>0.62714119407949398</v>
-      </c>
-      <c r="C42">
-        <v>0.66012637179913503</v>
-      </c>
-      <c r="D42">
-        <v>0.61934477379095099</v>
-      </c>
-      <c r="E42">
-        <v>0.63908564069542795</v>
-      </c>
-      <c r="F42">
-        <v>0.62709294244013403</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
-        <v>701</v>
-      </c>
-      <c r="B43">
-        <v>0.62431398636288005</v>
-      </c>
-      <c r="C43">
-        <v>0.55404057199866896</v>
-      </c>
-      <c r="D43">
-        <v>0.64473684210526305</v>
-      </c>
-      <c r="E43">
-        <v>0.59595778930423804</v>
-      </c>
-      <c r="F43">
-        <v>0.62429738439631199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
-        <v>801</v>
-      </c>
-      <c r="B44">
-        <v>0.634458672875436</v>
-      </c>
-      <c r="C44">
-        <v>0.61157299634186901</v>
-      </c>
-      <c r="D44">
-        <v>0.64098989194841405</v>
-      </c>
-      <c r="E44">
-        <v>0.62593601089176298</v>
-      </c>
-      <c r="F44">
-        <v>0.63488227577159395</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
-        <v>901</v>
-      </c>
-      <c r="B45">
-        <v>0.63894894395476398</v>
-      </c>
-      <c r="C45">
-        <v>0.60226139008978996</v>
-      </c>
-      <c r="D45">
-        <v>0.650035893754486</v>
-      </c>
-      <c r="E45">
-        <v>0.62523735542896597</v>
-      </c>
-      <c r="F45">
-        <v>0.63988410713023802</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
-        <v>1001</v>
-      </c>
-      <c r="B46">
-        <v>0.58040911358722702</v>
-      </c>
-      <c r="C46">
-        <v>0.27302959760558698</v>
-      </c>
-      <c r="D46">
-        <v>0.70898100172711498</v>
-      </c>
-      <c r="E46">
-        <v>0.39423769507803103</v>
-      </c>
-      <c r="F46">
         <v>0.53737400183270001</v>
       </c>
     </row>

</xml_diff>